<commit_message>
Appended backlog with some estimates; added few smaller tasks (fixture creation); added order creation & email notifications to feature set
</commit_message>
<xml_diff>
--- a/Sprint-2-Backlog.xlsx
+++ b/Sprint-2-Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>Sprint #2 Backlog</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Edit account information (where applicable)</t>
-  </si>
-  <si>
-    <t>Edit restaurant information</t>
   </si>
   <si>
     <t>Employee</t>
@@ -299,19 +296,39 @@
       <t>(a, b, c)</t>
     </r>
   </si>
+  <si>
+    <t>Estimate (hrs)</t>
+  </si>
+  <si>
+    <t>Luke</t>
+  </si>
+  <si>
+    <t>Create new food items (belong to a restaurant's menu)</t>
+  </si>
+  <si>
+    <t>An employee should be able to create new food items for her restaurant's menu.  When successfully saved to the system, restaurants' items are displayed in some logical manner (depicting a menu) where students view the restaurant's details.</t>
+  </si>
+  <si>
+    <t>A student should be able to create an order by adding food items (from single restaurant) to an order.  After submitting the order, she should receive an email (similar to a receipt) with order details. When the order is complete, she should receive a second email notification.  She should not be able to place an order if she already has a pending order in the system.</t>
+  </si>
+  <si>
+    <t>Restaurant Employee Fixtures</t>
+  </si>
+  <si>
+    <t>Administrator Fixtures</t>
+  </si>
+  <si>
+    <t>Food Item Fixtures</t>
+  </si>
+  <si>
+    <t>Order Fixtures</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -532,59 +549,77 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -914,42 +949,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="57.1640625" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" customWidth="1"/>
     <col min="4" max="4" width="21.83203125" customWidth="1"/>
     <col min="5" max="5" width="88.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="9"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:8" ht="28" customHeight="1" thickBot="1">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
@@ -965,21 +1000,24 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="14"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="40" customHeight="1">
       <c r="A9" s="3" t="s">
@@ -988,10 +1026,14 @@
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="15" t="s">
-        <v>26</v>
+      <c r="C9" s="17">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -1001,100 +1043,126 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="15" t="s">
-        <v>16</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="40" customHeight="1">
       <c r="A11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="17">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="15" t="s">
-        <v>18</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="40" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="15" t="s">
-        <v>25</v>
+      <c r="C12" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="40" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="15" t="s">
-        <v>24</v>
+      <c r="C13" s="17">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:8" ht="40" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="15"/>
+        <v>9</v>
+      </c>
+      <c r="C14" s="17">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:8" ht="40" customHeight="1">
+    <row r="15" spans="1:8" ht="79" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="C15" s="17">
+        <v>3</v>
+      </c>
       <c r="D15" s="3"/>
-      <c r="E15" s="15" t="s">
-        <v>20</v>
+      <c r="E15" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="40" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="17">
+        <v>1.5</v>
+      </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="15" t="s">
-        <v>21</v>
+      <c r="E16" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -1106,176 +1174,206 @@
       <c r="B17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="3"/>
+      <c r="C17" s="17"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="15"/>
+      <c r="E17" s="6"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="40" customHeight="1">
+    <row r="18" spans="1:7" ht="52" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="C18" s="17">
+        <v>2</v>
+      </c>
       <c r="D18" s="3"/>
-      <c r="E18" s="15"/>
+      <c r="E18" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" ht="40" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="C19" s="17">
+        <v>1</v>
+      </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="15"/>
+      <c r="E19" s="6"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" ht="40" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="17"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="15"/>
+      <c r="E20" s="6"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" ht="40" customHeight="1">
       <c r="A21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="17"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="15" t="s">
-        <v>32</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" ht="40" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="3"/>
+      <c r="C22" s="17"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="15"/>
+      <c r="E22" s="6"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" ht="40" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="3"/>
+      <c r="C23" s="17"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="15"/>
+      <c r="E23" s="6"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" ht="40" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="3"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="15"/>
+      <c r="E24" s="6"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" ht="40" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="3"/>
+      <c r="C25" s="17"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="15"/>
+      <c r="E25" s="6"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" ht="40" customHeight="1">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
+      <c r="A26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="17">
+        <v>0.5</v>
+      </c>
       <c r="D26" s="3"/>
-      <c r="E26" s="15"/>
+      <c r="E26" s="6"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" ht="40" customHeight="1">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
+      <c r="A27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="17">
+        <v>0.5</v>
+      </c>
       <c r="D27" s="3"/>
-      <c r="E27" s="15"/>
+      <c r="E27" s="6"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" ht="40" customHeight="1">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
+      <c r="A28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="17">
+        <v>0.5</v>
+      </c>
       <c r="D28" s="3"/>
-      <c r="E28" s="15"/>
+      <c r="E28" s="6"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" ht="36" customHeight="1">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="A29" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="17">
+        <v>0.5</v>
+      </c>
       <c r="D29" s="3"/>
-      <c r="E29" s="15"/>
+      <c r="E29" s="6"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" ht="36" customHeight="1">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
+      <c r="C30" s="17"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="16"/>
+      <c r="E30" s="7"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" ht="18">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
+      <c r="C31" s="17"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="16"/>
+      <c r="E31" s="7"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:7" ht="18">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
+      <c r="C32" s="17"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -1284,7 +1382,7 @@
     <row r="33" spans="1:7" ht="18">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
+      <c r="C33" s="17"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -1293,11 +1391,23 @@
     <row r="34" spans="1:7" ht="18">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
+      <c r="C34" s="17"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="C35" s="18"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="C36" s="18"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="C37" s="18"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="C38" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Setting up dynamic rendering of homepage (student vs. admin); updating backlog
</commit_message>
<xml_diff>
--- a/Sprint-2-Backlog.xlsx
+++ b/Sprint-2-Backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23260" windowHeight="13180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -959,20 +959,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="57.19921875" customWidth="1"/>
-    <col min="2" max="2" width="19.796875" customWidth="1"/>
-    <col min="3" max="3" width="29.19921875" customWidth="1"/>
-    <col min="4" max="4" width="21.796875" customWidth="1"/>
+    <col min="1" max="1" width="57.1640625" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" customWidth="1"/>
     <col min="5" max="5" width="88.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -980,13 +980,13 @@
       <c r="C1" s="11"/>
       <c r="D1" s="12"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15" customHeight="1">
       <c r="A2" s="13"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="15"/>
     </row>
-    <row r="3" spans="1:8" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="28" customHeight="1" thickBot="1">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -994,13 +994,13 @@
       <c r="C3" s="17"/>
       <c r="D3" s="18"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="37.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:8" s="1" customFormat="1" ht="43.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" ht="37" customHeight="1"/>
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="43" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1027,7 +1027,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="40" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -1046,7 +1046,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="40" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -1065,7 +1065,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="40" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -1084,7 +1084,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="40" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -1103,7 +1103,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="40" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
@@ -1122,7 +1122,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="40" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
@@ -1141,7 +1141,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:8" ht="79.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="79" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
@@ -1151,16 +1151,14 @@
       <c r="C15" s="8">
         <v>3</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="D15" s="3"/>
       <c r="E15" s="6" t="s">
         <v>40</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="40" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -1177,7 +1175,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="40" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
@@ -1190,7 +1188,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="52.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="52" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>38</v>
       </c>
@@ -1209,7 +1207,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="40" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
@@ -1226,7 +1224,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="40" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
@@ -1241,7 +1239,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="40" customHeight="1">
       <c r="A21" s="3" t="s">
         <v>29</v>
       </c>
@@ -1256,7 +1254,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="40" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>32</v>
       </c>
@@ -1271,7 +1269,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="40" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>33</v>
       </c>
@@ -1286,7 +1284,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="40" customHeight="1">
       <c r="A24" s="3" t="s">
         <v>34</v>
       </c>
@@ -1301,7 +1299,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="40" customHeight="1">
       <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
@@ -1316,7 +1314,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="40" customHeight="1">
       <c r="A26" s="3" t="s">
         <v>41</v>
       </c>
@@ -1331,7 +1329,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="40" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>42</v>
       </c>
@@ -1341,12 +1339,14 @@
       <c r="C27" s="8">
         <v>0.5</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="E27" s="6"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="40" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>43</v>
       </c>
@@ -1361,7 +1361,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="36" customHeight="1">
       <c r="A29" s="3" t="s">
         <v>44</v>
       </c>
@@ -1376,7 +1376,7 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="36" customHeight="1">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="8"/>
@@ -1385,7 +1385,7 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="18">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="8"/>
@@ -1394,7 +1394,7 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="18">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="8"/>
@@ -1403,7 +1403,7 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="18">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="8"/>
@@ -1412,7 +1412,7 @@
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="18">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="8"/>
@@ -1421,16 +1421,16 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7">
       <c r="C35" s="9"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7">
       <c r="C36" s="9"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7">
       <c r="C37" s="9"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7">
       <c r="C38" s="9"/>
     </row>
   </sheetData>

</xml_diff>